<commit_message>
Updated Python Excel Files
Files for Python Regression with appropriate variable names
</commit_message>
<xml_diff>
--- a/US-India_for_Python.xlsx
+++ b/US-India_for_Python.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizne\OneDrive\Desktop\Regression Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizne\OneDrive\Desktop\Fall 2021\Regression Project\Our Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B797F59-503F-4DBF-BE39-ABC9162B7D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB4470-7155-49FD-BA5E-BD30BB527052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2592" yWindow="852" windowWidth="19536" windowHeight="11496" xr2:uid="{88ADA460-7F97-48F3-A7B0-14646476B47D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88ADA460-7F97-48F3-A7B0-14646476B47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="26">
   <si>
     <t>IND_M</t>
   </si>
@@ -72,31 +72,13 @@
     <t>IND_Ln_VOL</t>
   </si>
   <si>
-    <t>Capitalgoods</t>
-  </si>
-  <si>
-    <t>Consumergoods</t>
-  </si>
-  <si>
-    <t>Intermediategoods</t>
-  </si>
-  <si>
-    <t>Rawmaterials</t>
-  </si>
-  <si>
     <t>Chemicals</t>
   </si>
   <si>
     <t>Fuels</t>
   </si>
   <si>
-    <t>MachandElec</t>
-  </si>
-  <si>
     <t>Metals</t>
-  </si>
-  <si>
-    <t>PlasticorRubber</t>
   </si>
   <si>
     <t>Transportation</t>
@@ -109,6 +91,27 @@
   </si>
   <si>
     <t>IND_Ln_Y_US</t>
+  </si>
+  <si>
+    <t>Capital Goods</t>
+  </si>
+  <si>
+    <t>Consumer Goods</t>
+  </si>
+  <si>
+    <t>Intermediate Goods</t>
+  </si>
+  <si>
+    <t>Raw Materials</t>
+  </si>
+  <si>
+    <t>Plastic or Rubber</t>
+  </si>
+  <si>
+    <t>Commodities</t>
+  </si>
+  <si>
+    <t>Mechanical and Electrical Goods</t>
   </si>
 </sst>
 </file>
@@ -532,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE8FB62-092C-45CF-AF32-41D70B17A8B0}">
   <dimension ref="A1:R970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J247" workbookViewId="0">
-      <selection activeCell="K247" sqref="K247"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>6</v>
@@ -588,16 +591,16 @@
         <v>9</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>10</v>
@@ -614,7 +617,7 @@
         <v>1088706.6100000001</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" s="13">
         <v>1</v>
@@ -642,7 +645,7 @@
         <v>6.04</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N2" s="13">
         <v>1994</v>
@@ -668,7 +671,7 @@
         <v>214171.45</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" s="13">
         <v>2</v>
@@ -696,7 +699,7 @@
         <v>5.33</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N3" s="13">
         <v>1994</v>
@@ -722,7 +725,7 @@
         <v>714851.64</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D4" s="13">
         <v>3</v>
@@ -750,7 +753,7 @@
         <v>5.85</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N4" s="13">
         <v>1994</v>
@@ -776,7 +779,7 @@
         <v>200875.38</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D5" s="13">
         <v>4</v>
@@ -804,7 +807,7 @@
         <v>5.3</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N5" s="13">
         <v>1994</v>
@@ -830,7 +833,7 @@
         <v>372292.88</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="13">
         <v>5</v>
@@ -858,7 +861,7 @@
         <v>5.57</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N6" s="13">
         <v>1994</v>
@@ -884,7 +887,7 @@
         <v>43438.96</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" s="13">
         <v>6</v>
@@ -912,7 +915,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N7" s="13">
         <v>1994</v>
@@ -938,7 +941,7 @@
         <v>730665.57</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D8" s="13">
         <v>7</v>
@@ -966,7 +969,7 @@
         <v>5.86</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N8" s="13">
         <v>1994</v>
@@ -992,7 +995,7 @@
         <v>163427</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D9" s="13">
         <v>8</v>
@@ -1020,7 +1023,7 @@
         <v>5.21</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N9" s="13">
         <v>1994</v>
@@ -1046,7 +1049,7 @@
         <v>61374.38</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="13">
         <v>9</v>
@@ -1074,7 +1077,7 @@
         <v>4.79</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N10" s="13">
         <v>1994</v>
@@ -1100,7 +1103,7 @@
         <v>366414.23</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D11" s="13">
         <v>10</v>
@@ -1128,7 +1131,7 @@
         <v>5.56</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N11" s="13">
         <v>1994</v>
@@ -1154,7 +1157,7 @@
         <v>1449993</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D12" s="13">
         <v>1</v>
@@ -1182,7 +1185,7 @@
         <v>6.16</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N12" s="13">
         <v>1995</v>
@@ -1208,7 +1211,7 @@
         <v>307980.13</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D13" s="13">
         <v>2</v>
@@ -1236,7 +1239,7 @@
         <v>5.49</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N13" s="13">
         <v>1995</v>
@@ -1262,7 +1265,7 @@
         <v>1063473.04</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14" s="13">
         <v>3</v>
@@ -1290,7 +1293,7 @@
         <v>6.03</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N14" s="13">
         <v>1995</v>
@@ -1316,7 +1319,7 @@
         <v>349868.9</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D15" s="13">
         <v>4</v>
@@ -1344,7 +1347,7 @@
         <v>5.54</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N15" s="13">
         <v>1995</v>
@@ -1370,7 +1373,7 @@
         <v>577588.21</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16" s="13">
         <v>5</v>
@@ -1398,7 +1401,7 @@
         <v>5.76</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N16" s="13">
         <v>1995</v>
@@ -1424,7 +1427,7 @@
         <v>80666.600000000006</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D17" s="13">
         <v>6</v>
@@ -1452,7 +1455,7 @@
         <v>4.91</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N17" s="13">
         <v>1995</v>
@@ -1478,7 +1481,7 @@
         <v>1248708.96</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D18" s="13">
         <v>7</v>
@@ -1506,7 +1509,7 @@
         <v>6.1</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N18" s="13">
         <v>1995</v>
@@ -1532,7 +1535,7 @@
         <v>276524.01</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D19" s="13">
         <v>8</v>
@@ -1560,7 +1563,7 @@
         <v>5.44</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N19" s="13">
         <v>1995</v>
@@ -1586,7 +1589,7 @@
         <v>105371.07</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D20" s="13">
         <v>9</v>
@@ -1614,7 +1617,7 @@
         <v>5.0199999999999996</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N20" s="13">
         <v>1995</v>
@@ -1640,7 +1643,7 @@
         <v>229201.24</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D21" s="13">
         <v>10</v>
@@ -1668,7 +1671,7 @@
         <v>5.36</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N21" s="13">
         <v>1995</v>
@@ -1694,7 +1697,7 @@
         <v>1832813.44</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D22" s="13">
         <v>1</v>
@@ -1722,7 +1725,7 @@
         <v>6.26</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N22" s="13">
         <v>1996</v>
@@ -1748,7 +1751,7 @@
         <v>308866.23</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -1776,7 +1779,7 @@
         <v>5.49</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N23" s="13">
         <v>1996</v>
@@ -1802,7 +1805,7 @@
         <v>865196.82</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D24" s="13">
         <v>3</v>
@@ -1830,7 +1833,7 @@
         <v>5.94</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N24" s="13">
         <v>1996</v>
@@ -1856,7 +1859,7 @@
         <v>197260.55</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D25" s="13">
         <v>4</v>
@@ -1884,7 +1887,7 @@
         <v>5.3</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N25" s="13">
         <v>1996</v>
@@ -1910,7 +1913,7 @@
         <v>377130.49</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D26" s="13">
         <v>5</v>
@@ -1938,7 +1941,7 @@
         <v>5.58</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N26" s="13">
         <v>1996</v>
@@ -1964,7 +1967,7 @@
         <v>66166.990000000005</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D27" s="13">
         <v>6</v>
@@ -1992,7 +1995,7 @@
         <v>4.82</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N27" s="13">
         <v>1996</v>
@@ -2018,7 +2021,7 @@
         <v>1283446.18</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D28" s="13">
         <v>7</v>
@@ -2046,7 +2049,7 @@
         <v>6.11</v>
       </c>
       <c r="M28" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N28" s="13">
         <v>1996</v>
@@ -2072,7 +2075,7 @@
         <v>221151.15</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D29" s="13">
         <v>8</v>
@@ -2100,7 +2103,7 @@
         <v>5.34</v>
       </c>
       <c r="M29" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N29" s="13">
         <v>1996</v>
@@ -2126,7 +2129,7 @@
         <v>121041.24</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D30" s="13">
         <v>9</v>
@@ -2154,7 +2157,7 @@
         <v>5.08</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N30" s="13">
         <v>1996</v>
@@ -2180,7 +2183,7 @@
         <v>542665.47</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D31" s="13">
         <v>10</v>
@@ -2208,7 +2211,7 @@
         <v>5.73</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N31" s="13">
         <v>1996</v>
@@ -2234,7 +2237,7 @@
         <v>1808211.16</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D32" s="13">
         <v>1</v>
@@ -2262,7 +2265,7 @@
         <v>6.26</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N32" s="13">
         <v>1997</v>
@@ -2288,7 +2291,7 @@
         <v>430166.24</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13">
         <v>2</v>
@@ -2316,7 +2319,7 @@
         <v>5.63</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N33" s="13">
         <v>1997</v>
@@ -2342,7 +2345,7 @@
         <v>1070350.46</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D34" s="13">
         <v>3</v>
@@ -2370,7 +2373,7 @@
         <v>6.03</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N34" s="13">
         <v>1997</v>
@@ -2396,7 +2399,7 @@
         <v>189300.27</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D35" s="13">
         <v>4</v>
@@ -2424,7 +2427,7 @@
         <v>5.28</v>
       </c>
       <c r="M35" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N35" s="13">
         <v>1997</v>
@@ -2450,7 +2453,7 @@
         <v>719408.05</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D36" s="13">
         <v>5</v>
@@ -2478,7 +2481,7 @@
         <v>5.86</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N36" s="13">
         <v>1997</v>
@@ -2504,7 +2507,7 @@
         <v>69223.100000000006</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D37" s="13">
         <v>6</v>
@@ -2532,7 +2535,7 @@
         <v>4.84</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N37" s="13">
         <v>1997</v>
@@ -2558,7 +2561,7 @@
         <v>1444083.71</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D38" s="13">
         <v>7</v>
@@ -2586,7 +2589,7 @@
         <v>6.16</v>
       </c>
       <c r="M38" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N38" s="13">
         <v>1997</v>
@@ -2612,7 +2615,7 @@
         <v>186805.03</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D39" s="13">
         <v>8</v>
@@ -2640,7 +2643,7 @@
         <v>5.27</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N39" s="13">
         <v>1997</v>
@@ -2666,7 +2669,7 @@
         <v>107533.59</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D40" s="13">
         <v>9</v>
@@ -2694,7 +2697,7 @@
         <v>5.03</v>
       </c>
       <c r="M40" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N40" s="13">
         <v>1997</v>
@@ -2720,7 +2723,7 @@
         <v>312110.73</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D41" s="13">
         <v>10</v>
@@ -2748,7 +2751,7 @@
         <v>5.49</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N41" s="13">
         <v>1997</v>
@@ -2774,7 +2777,7 @@
         <v>1788136.01</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D42" s="13">
         <v>1</v>
@@ -2802,7 +2805,7 @@
         <v>6.25</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N42" s="13">
         <v>1998</v>
@@ -2828,7 +2831,7 @@
         <v>364407.7</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D43" s="13">
         <v>2</v>
@@ -2856,7 +2859,7 @@
         <v>5.56</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N43" s="13">
         <v>1998</v>
@@ -2882,7 +2885,7 @@
         <v>1104741.32</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D44" s="13">
         <v>3</v>
@@ -2910,7 +2913,7 @@
         <v>6.04</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N44" s="13">
         <v>1998</v>
@@ -2936,7 +2939,7 @@
         <v>184014.9</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D45" s="13">
         <v>4</v>
@@ -2964,7 +2967,7 @@
         <v>5.26</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N45" s="13">
         <v>1998</v>
@@ -2990,7 +2993,7 @@
         <v>725786.2</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D46" s="13">
         <v>5</v>
@@ -3018,7 +3021,7 @@
         <v>5.86</v>
       </c>
       <c r="M46" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N46" s="13">
         <v>1998</v>
@@ -3044,7 +3047,7 @@
         <v>52071.07</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D47" s="13">
         <v>6</v>
@@ -3072,7 +3075,7 @@
         <v>4.72</v>
       </c>
       <c r="M47" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N47" s="13">
         <v>1998</v>
@@ -3098,7 +3101,7 @@
         <v>1209427.3</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D48" s="13">
         <v>7</v>
@@ -3126,7 +3129,7 @@
         <v>6.08</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N48" s="13">
         <v>1998</v>
@@ -3152,7 +3155,7 @@
         <v>132429.47</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D49" s="13">
         <v>8</v>
@@ -3180,7 +3183,7 @@
         <v>5.12</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N49" s="13">
         <v>1998</v>
@@ -3206,7 +3209,7 @@
         <v>81902.399999999994</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D50" s="13">
         <v>9</v>
@@ -3234,7 +3237,7 @@
         <v>4.91</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N50" s="13">
         <v>1998</v>
@@ -3260,7 +3263,7 @@
         <v>502327.81</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D51" s="13">
         <v>10</v>
@@ -3288,7 +3291,7 @@
         <v>5.7</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N51" s="13">
         <v>1998</v>
@@ -3314,7 +3317,7 @@
         <v>1743075.5</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D52" s="13">
         <v>1</v>
@@ -3342,7 +3345,7 @@
         <v>6.24</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N52" s="13">
         <v>1999</v>
@@ -3368,7 +3371,7 @@
         <v>347512.36</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D53" s="13">
         <v>2</v>
@@ -3396,7 +3399,7 @@
         <v>5.54</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N53" s="13">
         <v>1999</v>
@@ -3422,7 +3425,7 @@
         <v>1295399.03</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D54" s="13">
         <v>3</v>
@@ -3450,7 +3453,7 @@
         <v>6.11</v>
       </c>
       <c r="M54" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N54" s="13">
         <v>1999</v>
@@ -3476,7 +3479,7 @@
         <v>194233.59</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D55" s="13">
         <v>4</v>
@@ -3504,7 +3507,7 @@
         <v>5.29</v>
       </c>
       <c r="M55" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N55" s="13">
         <v>1999</v>
@@ -3530,7 +3533,7 @@
         <v>839994.02</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D56" s="13">
         <v>5</v>
@@ -3558,7 +3561,7 @@
         <v>5.92</v>
       </c>
       <c r="M56" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N56" s="13">
         <v>1999</v>
@@ -3584,7 +3587,7 @@
         <v>52605.14</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D57" s="13">
         <v>6</v>
@@ -3612,7 +3615,7 @@
         <v>4.72</v>
       </c>
       <c r="M57" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N57" s="13">
         <v>1999</v>
@@ -3638,7 +3641,7 @@
         <v>1090450.18</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D58" s="13">
         <v>7</v>
@@ -3666,7 +3669,7 @@
         <v>6.04</v>
       </c>
       <c r="M58" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N58" s="13">
         <v>1999</v>
@@ -3692,7 +3695,7 @@
         <v>133992.07</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D59" s="13">
         <v>8</v>
@@ -3720,7 +3723,7 @@
         <v>5.13</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N59" s="13">
         <v>1999</v>
@@ -3746,7 +3749,7 @@
         <v>93002.53</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D60" s="13">
         <v>9</v>
@@ -3774,7 +3777,7 @@
         <v>4.97</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N60" s="13">
         <v>1999</v>
@@ -3800,7 +3803,7 @@
         <v>567100.64</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D61" s="13">
         <v>10</v>
@@ -3828,7 +3831,7 @@
         <v>5.75</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N61" s="13">
         <v>1999</v>
@@ -3854,7 +3857,7 @@
         <v>1822643.89</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D62" s="13">
         <v>1</v>
@@ -3882,7 +3885,7 @@
         <v>6.26</v>
       </c>
       <c r="M62" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N62" s="13">
         <v>2000</v>
@@ -3908,7 +3911,7 @@
         <v>489287.87</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D63" s="13">
         <v>2</v>
@@ -3936,7 +3939,7 @@
         <v>5.69</v>
       </c>
       <c r="M63" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N63" s="13">
         <v>2000</v>
@@ -3962,7 +3965,7 @@
         <v>916738.85</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D64" s="13">
         <v>3</v>
@@ -3990,7 +3993,7 @@
         <v>5.96</v>
       </c>
       <c r="M64" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N64" s="13">
         <v>2000</v>
@@ -4016,7 +4019,7 @@
         <v>255505.71</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D65" s="13">
         <v>4</v>
@@ -4044,7 +4047,7 @@
         <v>5.41</v>
       </c>
       <c r="M65" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N65" s="13">
         <v>2000</v>
@@ -4070,7 +4073,7 @@
         <v>462522.4</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D66" s="13">
         <v>5</v>
@@ -4098,7 +4101,7 @@
         <v>5.67</v>
       </c>
       <c r="M66" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N66" s="13">
         <v>2000</v>
@@ -4124,7 +4127,7 @@
         <v>82698.259999999995</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D67" s="13">
         <v>6</v>
@@ -4152,7 +4155,7 @@
         <v>4.92</v>
       </c>
       <c r="M67" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N67" s="13">
         <v>2000</v>
@@ -4178,7 +4181,7 @@
         <v>1475696.44</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D68" s="13">
         <v>7</v>
@@ -4206,7 +4209,7 @@
         <v>6.17</v>
       </c>
       <c r="M68" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N68" s="13">
         <v>2000</v>
@@ -4232,7 +4235,7 @@
         <v>156954.01999999999</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D69" s="13">
         <v>8</v>
@@ -4260,7 +4263,7 @@
         <v>5.2</v>
       </c>
       <c r="M69" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N69" s="13">
         <v>2000</v>
@@ -4286,7 +4289,7 @@
         <v>87042.36</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D70" s="13">
         <v>9</v>
@@ -4314,7 +4317,7 @@
         <v>4.9400000000000004</v>
       </c>
       <c r="M70" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N70" s="13">
         <v>2000</v>
@@ -4340,7 +4343,7 @@
         <v>337958.17</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D71" s="13">
         <v>10</v>
@@ -4368,7 +4371,7 @@
         <v>5.53</v>
       </c>
       <c r="M71" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N71" s="13">
         <v>2000</v>
@@ -4394,7 +4397,7 @@
         <v>1729038.34</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D72" s="13">
         <v>1</v>
@@ -4422,7 +4425,7 @@
         <v>6.24</v>
       </c>
       <c r="M72" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N72" s="13">
         <v>2001</v>
@@ -4448,7 +4451,7 @@
         <v>498850.55</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D73" s="13">
         <v>2</v>
@@ -4476,7 +4479,7 @@
         <v>5.7</v>
       </c>
       <c r="M73" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N73" s="13">
         <v>2001</v>
@@ -4502,7 +4505,7 @@
         <v>905254.52</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D74" s="13">
         <v>3</v>
@@ -4530,7 +4533,7 @@
         <v>5.96</v>
       </c>
       <c r="M74" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N74" s="13">
         <v>2001</v>
@@ -4556,7 +4559,7 @@
         <v>444597.97</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D75" s="13">
         <v>4</v>
@@ -4584,7 +4587,7 @@
         <v>5.65</v>
       </c>
       <c r="M75" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N75" s="13">
         <v>2001</v>
@@ -4610,7 +4613,7 @@
         <v>436854.8</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D76" s="13">
         <v>5</v>
@@ -4638,7 +4641,7 @@
         <v>5.64</v>
       </c>
       <c r="M76" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N76" s="13">
         <v>2001</v>
@@ -4664,7 +4667,7 @@
         <v>84747.94</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D77" s="13">
         <v>6</v>
@@ -4692,7 +4695,7 @@
         <v>4.93</v>
       </c>
       <c r="M77" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N77" s="13">
         <v>2001</v>
@@ -4718,7 +4721,7 @@
         <v>1261519.2</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D78" s="13">
         <v>7</v>
@@ -4746,7 +4749,7 @@
         <v>6.1</v>
       </c>
       <c r="M78" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N78" s="13">
         <v>2001</v>
@@ -4772,7 +4775,7 @@
         <v>160082.99</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D79" s="13">
         <v>8</v>
@@ -4800,7 +4803,7 @@
         <v>5.2</v>
       </c>
       <c r="M79" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N79" s="13">
         <v>2001</v>
@@ -4826,7 +4829,7 @@
         <v>91278.6</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D80" s="13">
         <v>9</v>
@@ -4854,7 +4857,7 @@
         <v>4.96</v>
       </c>
       <c r="M80" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N80" s="13">
         <v>2001</v>
@@ -4880,7 +4883,7 @@
         <v>413828.35</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D81" s="13">
         <v>10</v>
@@ -4908,7 +4911,7 @@
         <v>5.62</v>
       </c>
       <c r="M81" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N81" s="13">
         <v>2001</v>
@@ -4934,7 +4937,7 @@
         <v>1896704.04</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D82" s="13">
         <v>1</v>
@@ -4962,7 +4965,7 @@
         <v>6.28</v>
       </c>
       <c r="M82" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N82" s="13">
         <v>2002</v>
@@ -4988,7 +4991,7 @@
         <v>706547.79</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D83" s="13">
         <v>2</v>
@@ -5016,7 +5019,7 @@
         <v>5.85</v>
       </c>
       <c r="M83" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N83" s="13">
         <v>2002</v>
@@ -5042,7 +5045,7 @@
         <v>1028673.52</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D84" s="13">
         <v>3</v>
@@ -5070,7 +5073,7 @@
         <v>6.01</v>
       </c>
       <c r="M84" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N84" s="13">
         <v>2002</v>
@@ -5096,7 +5099,7 @@
         <v>348991.18</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D85" s="13">
         <v>4</v>
@@ -5124,7 +5127,7 @@
         <v>5.54</v>
       </c>
       <c r="M85" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N85" s="13">
         <v>2002</v>
@@ -5150,7 +5153,7 @@
         <v>662802</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D86" s="13">
         <v>5</v>
@@ -5178,7 +5181,7 @@
         <v>5.82</v>
       </c>
       <c r="M86" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N86" s="13">
         <v>2002</v>
@@ -5204,7 +5207,7 @@
         <v>54173.7</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D87" s="13">
         <v>6</v>
@@ -5232,7 +5235,7 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="M87" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N87" s="13">
         <v>2002</v>
@@ -5258,7 +5261,7 @@
         <v>1494898.42</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D88" s="13">
         <v>7</v>
@@ -5286,7 +5289,7 @@
         <v>6.17</v>
       </c>
       <c r="M88" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N88" s="13">
         <v>2002</v>
@@ -5312,7 +5315,7 @@
         <v>155005.18</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D89" s="13">
         <v>8</v>
@@ -5340,7 +5343,7 @@
         <v>5.19</v>
       </c>
       <c r="M89" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N89" s="13">
         <v>2002</v>
@@ -5366,7 +5369,7 @@
         <v>125436.37</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D90" s="13">
         <v>9</v>
@@ -5394,7 +5397,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="M90" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N90" s="13">
         <v>2002</v>
@@ -5420,7 +5423,7 @@
         <v>367120.64000000001</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D91" s="13">
         <v>10</v>
@@ -5448,7 +5451,7 @@
         <v>5.56</v>
       </c>
       <c r="M91" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N91" s="13">
         <v>2002</v>
@@ -5474,7 +5477,7 @@
         <v>2120499.1800000002</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D92" s="13">
         <v>1</v>
@@ -5502,7 +5505,7 @@
         <v>6.33</v>
       </c>
       <c r="M92" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N92" s="13">
         <v>2003</v>
@@ -5528,7 +5531,7 @@
         <v>1004396.15</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D93" s="13">
         <v>2</v>
@@ -5556,7 +5559,7 @@
         <v>6</v>
       </c>
       <c r="M93" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N93" s="13">
         <v>2003</v>
@@ -5582,7 +5585,7 @@
         <v>1181866.97</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D94" s="13">
         <v>3</v>
@@ -5610,7 +5613,7 @@
         <v>6.07</v>
       </c>
       <c r="M94" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N94" s="13">
         <v>2003</v>
@@ -5636,7 +5639,7 @@
         <v>468637.22</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D95" s="13">
         <v>4</v>
@@ -5664,7 +5667,7 @@
         <v>5.67</v>
       </c>
       <c r="M95" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N95" s="13">
         <v>2003</v>
@@ -5690,7 +5693,7 @@
         <v>922187.08</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D96" s="13">
         <v>5</v>
@@ -5718,7 +5721,7 @@
         <v>5.96</v>
       </c>
       <c r="M96" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N96" s="13">
         <v>2003</v>
@@ -5744,7 +5747,7 @@
         <v>134289.38</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D97" s="13">
         <v>6</v>
@@ -5772,7 +5775,7 @@
         <v>5.13</v>
       </c>
       <c r="M97" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N97" s="13">
         <v>2003</v>
@@ -5798,7 +5801,7 @@
         <v>1640989.04</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D98" s="13">
         <v>7</v>
@@ -5826,7 +5829,7 @@
         <v>6.22</v>
       </c>
       <c r="M98" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N98" s="13">
         <v>2003</v>
@@ -5852,7 +5855,7 @@
         <v>185739.42</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D99" s="13">
         <v>8</v>
@@ -5880,7 +5883,7 @@
         <v>5.27</v>
       </c>
       <c r="M99" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N99" s="13">
         <v>2003</v>
@@ -5906,7 +5909,7 @@
         <v>151340.53</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D100" s="13">
         <v>9</v>
@@ -5934,7 +5937,7 @@
         <v>5.18</v>
       </c>
       <c r="M100" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N100" s="13">
         <v>2003</v>
@@ -5960,7 +5963,7 @@
         <v>389586.34</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D101" s="13">
         <v>10</v>
@@ -5988,7 +5991,7 @@
         <v>5.59</v>
       </c>
       <c r="M101" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N101" s="13">
         <v>2003</v>
@@ -6014,7 +6017,7 @@
         <v>2391491.7000000002</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D102" s="13">
         <v>1</v>
@@ -6042,7 +6045,7 @@
         <v>6.38</v>
       </c>
       <c r="M102" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N102" s="13">
         <v>2004</v>
@@ -6068,7 +6071,7 @@
         <v>877557.16</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D103" s="13">
         <v>2</v>
@@ -6096,7 +6099,7 @@
         <v>5.94</v>
       </c>
       <c r="M103" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N103" s="13">
         <v>2004</v>
@@ -6122,7 +6125,7 @@
         <v>1616931.46</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D104" s="13">
         <v>3</v>
@@ -6150,7 +6153,7 @@
         <v>6.21</v>
       </c>
       <c r="M104" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N104" s="13">
         <v>2004</v>
@@ -6176,7 +6179,7 @@
         <v>575599.67000000004</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D105" s="13">
         <v>4</v>
@@ -6204,7 +6207,7 @@
         <v>5.76</v>
       </c>
       <c r="M105" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N105" s="13">
         <v>2004</v>
@@ -6230,7 +6233,7 @@
         <v>874790.86</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D106" s="13">
         <v>5</v>
@@ -6258,7 +6261,7 @@
         <v>5.94</v>
       </c>
       <c r="M106" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N106" s="13">
         <v>2004</v>
@@ -6284,7 +6287,7 @@
         <v>313695.61</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D107" s="13">
         <v>6</v>
@@ -6312,7 +6315,7 @@
         <v>5.5</v>
       </c>
       <c r="M107" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N107" s="13">
         <v>2004</v>
@@ -6338,7 +6341,7 @@
         <v>2031518.94</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D108" s="13">
         <v>7</v>
@@ -6366,7 +6369,7 @@
         <v>6.31</v>
       </c>
       <c r="M108" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N108" s="13">
         <v>2004</v>
@@ -6392,7 +6395,7 @@
         <v>312953.21999999997</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D109" s="13">
         <v>8</v>
@@ -6420,7 +6423,7 @@
         <v>5.5</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N109" s="13">
         <v>2004</v>
@@ -6446,7 +6449,7 @@
         <v>182202.52</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D110" s="13">
         <v>9</v>
@@ -6474,7 +6477,7 @@
         <v>5.26</v>
       </c>
       <c r="M110" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N110" s="13">
         <v>2004</v>
@@ -6500,7 +6503,7 @@
         <v>131255.76</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D111" s="13">
         <v>10</v>
@@ -6528,7 +6531,7 @@
         <v>5.12</v>
       </c>
       <c r="M111" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N111" s="13">
         <v>2004</v>
@@ -6554,7 +6557,7 @@
         <v>2868750.7</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D112" s="13">
         <v>1</v>
@@ -6582,7 +6585,7 @@
         <v>6.46</v>
       </c>
       <c r="M112" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N112" s="13">
         <v>2005</v>
@@ -6608,7 +6611,7 @@
         <v>967840.55</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D113" s="13">
         <v>2</v>
@@ -6636,7 +6639,7 @@
         <v>5.99</v>
       </c>
       <c r="M113" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N113" s="13">
         <v>2005</v>
@@ -6662,7 +6665,7 @@
         <v>1999684.85</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D114" s="13">
         <v>3</v>
@@ -6690,7 +6693,7 @@
         <v>6.3</v>
       </c>
       <c r="M114" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N114" s="13">
         <v>2005</v>
@@ -6716,7 +6719,7 @@
         <v>811019.3</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D115" s="13">
         <v>4</v>
@@ -6744,7 +6747,7 @@
         <v>5.91</v>
       </c>
       <c r="M115" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N115" s="13">
         <v>2005</v>
@@ -6770,7 +6773,7 @@
         <v>883949.67</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D116" s="13">
         <v>5</v>
@@ -6798,7 +6801,7 @@
         <v>5.95</v>
       </c>
       <c r="M116" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N116" s="13">
         <v>2005</v>
@@ -6824,7 +6827,7 @@
         <v>356326.09</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D117" s="13">
         <v>6</v>
@@ -6852,7 +6855,7 @@
         <v>5.55</v>
       </c>
       <c r="M117" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N117" s="13">
         <v>2005</v>
@@ -6878,7 +6881,7 @@
         <v>2352060.59</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D118" s="13">
         <v>7</v>
@@ -6906,7 +6909,7 @@
         <v>6.37</v>
       </c>
       <c r="M118" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N118" s="13">
         <v>2005</v>
@@ -6932,7 +6935,7 @@
         <v>574268.24</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D119" s="13">
         <v>8</v>
@@ -6960,7 +6963,7 @@
         <v>5.76</v>
       </c>
       <c r="M119" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N119" s="13">
         <v>2005</v>
@@ -6986,7 +6989,7 @@
         <v>274167.28000000003</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D120" s="13">
         <v>9</v>
@@ -7014,7 +7017,7 @@
         <v>5.44</v>
       </c>
       <c r="M120" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N120" s="13">
         <v>2005</v>
@@ -7040,7 +7043,7 @@
         <v>164507.17000000001</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D121" s="13">
         <v>10</v>
@@ -7068,7 +7071,7 @@
         <v>5.22</v>
       </c>
       <c r="M121" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N121" s="13">
         <v>2005</v>
@@ -7094,7 +7097,7 @@
         <v>4871455.96</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D122" s="13">
         <v>1</v>
@@ -7122,7 +7125,7 @@
         <v>6.69</v>
       </c>
       <c r="M122" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N122" s="13">
         <v>2006</v>
@@ -7148,7 +7151,7 @@
         <v>1124361.67</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D123" s="13">
         <v>2</v>
@@ -7176,7 +7179,7 @@
         <v>6.05</v>
       </c>
       <c r="M123" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N123" s="13">
         <v>2006</v>
@@ -7202,7 +7205,7 @@
         <v>2493432.79</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D124" s="13">
         <v>3</v>
@@ -7230,7 +7233,7 @@
         <v>6.4</v>
       </c>
       <c r="M124" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N124" s="13">
         <v>2006</v>
@@ -7256,7 +7259,7 @@
         <v>814275.94</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D125" s="13">
         <v>4</v>
@@ -7284,7 +7287,7 @@
         <v>5.91</v>
       </c>
       <c r="M125" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N125" s="13">
         <v>2006</v>
@@ -7310,7 +7313,7 @@
         <v>1027960.41</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D126" s="13">
         <v>5</v>
@@ -7338,7 +7341,7 @@
         <v>6.01</v>
       </c>
       <c r="M126" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N126" s="13">
         <v>2006</v>
@@ -7364,7 +7367,7 @@
         <v>396150.97</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D127" s="13">
         <v>6</v>
@@ -7392,7 +7395,7 @@
         <v>5.6</v>
       </c>
       <c r="M127" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N127" s="13">
         <v>2006</v>
@@ -7418,7 +7421,7 @@
         <v>2762207.34</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D128" s="13">
         <v>7</v>
@@ -7446,7 +7449,7 @@
         <v>6.44</v>
       </c>
       <c r="M128" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N128" s="13">
         <v>2006</v>
@@ -7472,7 +7475,7 @@
         <v>562301.89</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D129" s="13">
         <v>8</v>
@@ -7500,7 +7503,7 @@
         <v>5.75</v>
       </c>
       <c r="M129" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N129" s="13">
         <v>2006</v>
@@ -7526,7 +7529,7 @@
         <v>334693.96999999997</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D130" s="13">
         <v>9</v>
@@ -7554,7 +7557,7 @@
         <v>5.52</v>
       </c>
       <c r="M130" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N130" s="13">
         <v>2006</v>
@@ -7580,7 +7583,7 @@
         <v>1722640.07</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D131" s="13">
         <v>10</v>
@@ -7608,7 +7611,7 @@
         <v>6.24</v>
       </c>
       <c r="M131" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N131" s="13">
         <v>2006</v>
@@ -7634,7 +7637,7 @@
         <v>10155392.27</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D132" s="13">
         <v>1</v>
@@ -7662,7 +7665,7 @@
         <v>7.01</v>
       </c>
       <c r="M132" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N132" s="13">
         <v>2007</v>
@@ -7688,7 +7691,7 @@
         <v>1363606.77</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D133" s="13">
         <v>2</v>
@@ -7716,7 +7719,7 @@
         <v>6.13</v>
       </c>
       <c r="M133" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N133" s="13">
         <v>2007</v>
@@ -7742,7 +7745,7 @@
         <v>3903997.69</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D134" s="13">
         <v>3</v>
@@ -7770,7 +7773,7 @@
         <v>6.59</v>
       </c>
       <c r="M134" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N134" s="13">
         <v>2007</v>
@@ -7796,7 +7799,7 @@
         <v>1118132.56</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D135" s="13">
         <v>4</v>
@@ -7824,7 +7827,7 @@
         <v>6.05</v>
       </c>
       <c r="M135" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N135" s="13">
         <v>2007</v>
@@ -7850,7 +7853,7 @@
         <v>1217483</v>
       </c>
       <c r="C136" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D136" s="13">
         <v>5</v>
@@ -7878,7 +7881,7 @@
         <v>6.09</v>
       </c>
       <c r="M136" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N136" s="13">
         <v>2007</v>
@@ -7904,7 +7907,7 @@
         <v>398062.78</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D137" s="13">
         <v>6</v>
@@ -7932,7 +7935,7 @@
         <v>5.6</v>
       </c>
       <c r="M137" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N137" s="13">
         <v>2007</v>
@@ -7958,7 +7961,7 @@
         <v>3512901.57</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D138" s="13">
         <v>7</v>
@@ -7986,7 +7989,7 @@
         <v>6.55</v>
       </c>
       <c r="M138" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N138" s="13">
         <v>2007</v>
@@ -8012,7 +8015,7 @@
         <v>847438.25</v>
       </c>
       <c r="C139" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D139" s="13">
         <v>8</v>
@@ -8040,7 +8043,7 @@
         <v>5.93</v>
       </c>
       <c r="M139" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N139" s="13">
         <v>2007</v>
@@ -8066,7 +8069,7 @@
         <v>477802.3</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D140" s="13">
         <v>9</v>
@@ -8094,7 +8097,7 @@
         <v>5.68</v>
       </c>
       <c r="M140" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N140" s="13">
         <v>2007</v>
@@ -8120,7 +8123,7 @@
         <v>6203822.0300000003</v>
       </c>
       <c r="C141" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D141" s="13">
         <v>10</v>
@@ -8148,7 +8151,7 @@
         <v>6.79</v>
       </c>
       <c r="M141" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N141" s="13">
         <v>2007</v>
@@ -8174,7 +8177,7 @@
         <v>7147632.1500000004</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D142" s="13">
         <v>1</v>
@@ -8202,7 +8205,7 @@
         <v>6.85</v>
       </c>
       <c r="M142" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N142" s="13">
         <v>2008</v>
@@ -8228,7 +8231,7 @@
         <v>1376104.97</v>
       </c>
       <c r="C143" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D143" s="13">
         <v>2</v>
@@ -8256,7 +8259,7 @@
         <v>6.14</v>
       </c>
       <c r="M143" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N143" s="13">
         <v>2008</v>
@@ -8282,7 +8285,7 @@
         <v>8364690.5800000001</v>
       </c>
       <c r="C144" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D144" s="13">
         <v>3</v>
@@ -8310,7 +8313,7 @@
         <v>6.92</v>
       </c>
       <c r="M144" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N144" s="13">
         <v>2008</v>
@@ -8336,7 +8339,7 @@
         <v>1431440.25</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D145" s="13">
         <v>4</v>
@@ -8364,7 +8367,7 @@
         <v>6.16</v>
       </c>
       <c r="M145" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N145" s="13">
         <v>2008</v>
@@ -8390,7 +8393,7 @@
         <v>4457062.6399999997</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D146" s="13">
         <v>5</v>
@@ -8418,7 +8421,7 @@
         <v>6.65</v>
       </c>
       <c r="M146" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N146" s="13">
         <v>2008</v>
@@ -8444,7 +8447,7 @@
         <v>884442.09</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D147" s="13">
         <v>6</v>
@@ -8472,7 +8475,7 @@
         <v>5.95</v>
       </c>
       <c r="M147" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N147" s="13">
         <v>2008</v>
@@ -8498,7 +8501,7 @@
         <v>3774957.96</v>
       </c>
       <c r="C148" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D148" s="13">
         <v>7</v>
@@ -8526,7 +8529,7 @@
         <v>6.58</v>
       </c>
       <c r="M148" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N148" s="13">
         <v>2008</v>
@@ -8552,7 +8555,7 @@
         <v>969909.59</v>
       </c>
       <c r="C149" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D149" s="13">
         <v>8</v>
@@ -8580,7 +8583,7 @@
         <v>5.99</v>
       </c>
       <c r="M149" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N149" s="13">
         <v>2008</v>
@@ -8606,7 +8609,7 @@
         <v>624793.9</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D150" s="13">
         <v>9</v>
@@ -8634,7 +8637,7 @@
         <v>5.8</v>
       </c>
       <c r="M150" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N150" s="13">
         <v>2008</v>
@@ -8660,7 +8663,7 @@
         <v>2861762.27</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D151" s="13">
         <v>10</v>
@@ -8688,7 +8691,7 @@
         <v>6.46</v>
       </c>
       <c r="M151" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N151" s="13">
         <v>2008</v>
@@ -8714,7 +8717,7 @@
         <v>4542266.82</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D152" s="13">
         <v>1</v>
@@ -8742,7 +8745,7 @@
         <v>6.66</v>
       </c>
       <c r="M152" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N152" s="13">
         <v>2009</v>
@@ -8768,7 +8771,7 @@
         <v>1278527.81</v>
       </c>
       <c r="C153" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D153" s="13">
         <v>2</v>
@@ -8796,7 +8799,7 @@
         <v>6.11</v>
       </c>
       <c r="M153" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N153" s="13">
         <v>2009</v>
@@ -8822,7 +8825,7 @@
         <v>6603030.79</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D154" s="13">
         <v>3</v>
@@ -8850,7 +8853,7 @@
         <v>6.82</v>
       </c>
       <c r="M154" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N154" s="13">
         <v>2009</v>
@@ -8876,7 +8879,7 @@
         <v>1562621.92</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D155" s="13">
         <v>4</v>
@@ -8904,7 +8907,7 @@
         <v>6.19</v>
       </c>
       <c r="M155" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N155" s="13">
         <v>2009</v>
@@ -8930,7 +8933,7 @@
         <v>2778054.71</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D156" s="13">
         <v>5</v>
@@ -8958,7 +8961,7 @@
         <v>6.44</v>
       </c>
       <c r="M156" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N156" s="13">
         <v>2009</v>
@@ -8984,7 +8987,7 @@
         <v>959775.06</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D157" s="13">
         <v>6</v>
@@ -9012,7 +9015,7 @@
         <v>5.98</v>
       </c>
       <c r="M157" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N157" s="13">
         <v>2009</v>
@@ -9038,7 +9041,7 @@
         <v>3625670.81</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D158" s="13">
         <v>7</v>
@@ -9066,7 +9069,7 @@
         <v>6.56</v>
       </c>
       <c r="M158" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N158" s="13">
         <v>2009</v>
@@ -9092,7 +9095,7 @@
         <v>941191.24</v>
       </c>
       <c r="C159" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D159" s="13">
         <v>8</v>
@@ -9120,7 +9123,7 @@
         <v>5.97</v>
       </c>
       <c r="M159" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N159" s="13">
         <v>2009</v>
@@ -9146,7 +9149,7 @@
         <v>739317.04</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D160" s="13">
         <v>9</v>
@@ -9174,7 +9177,7 @@
         <v>5.87</v>
       </c>
       <c r="M160" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N160" s="13">
         <v>2009</v>
@@ -9200,7 +9203,7 @@
         <v>311349.67</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D161" s="13">
         <v>10</v>
@@ -9228,7 +9231,7 @@
         <v>5.49</v>
       </c>
       <c r="M161" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N161" s="13">
         <v>2009</v>
@@ -9254,7 +9257,7 @@
         <v>5172144.8899999997</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D162" s="13">
         <v>1</v>
@@ -9282,7 +9285,7 @@
         <v>6.71</v>
       </c>
       <c r="M162" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N162" s="13">
         <v>2010</v>
@@ -9308,7 +9311,7 @@
         <v>1503260.24</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D163" s="13">
         <v>2</v>
@@ -9336,7 +9339,7 @@
         <v>6.18</v>
       </c>
       <c r="M163" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N163" s="13">
         <v>2010</v>
@@ -9362,7 +9365,7 @@
         <v>9312409.5899999999</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D164" s="13">
         <v>3</v>
@@ -9390,7 +9393,7 @@
         <v>6.97</v>
       </c>
       <c r="M164" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N164" s="13">
         <v>2010</v>
@@ -9416,7 +9419,7 @@
         <v>1737433.17</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D165" s="13">
         <v>4</v>
@@ -9444,7 +9447,7 @@
         <v>6.24</v>
       </c>
       <c r="M165" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N165" s="13">
         <v>2010</v>
@@ -9470,7 +9473,7 @@
         <v>3232920.36</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D166" s="13">
         <v>5</v>
@@ -9498,7 +9501,7 @@
         <v>6.51</v>
       </c>
       <c r="M166" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N166" s="13">
         <v>2010</v>
@@ -9524,7 +9527,7 @@
         <v>1079943.8700000001</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D167" s="13">
         <v>6</v>
@@ -9552,7 +9555,7 @@
         <v>6.03</v>
       </c>
       <c r="M167" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N167" s="13">
         <v>2010</v>
@@ -9578,7 +9581,7 @@
         <v>4029747.69</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D168" s="13">
         <v>7</v>
@@ -9606,7 +9609,7 @@
         <v>6.61</v>
       </c>
       <c r="M168" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N168" s="13">
         <v>2010</v>
@@ -9632,7 +9635,7 @@
         <v>970404.64</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D169" s="13">
         <v>8</v>
@@ -9660,7 +9663,7 @@
         <v>5.99</v>
       </c>
       <c r="M169" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N169" s="13">
         <v>2010</v>
@@ -9686,7 +9689,7 @@
         <v>898435.48</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D170" s="13">
         <v>9</v>
@@ -9714,7 +9717,7 @@
         <v>5.95</v>
       </c>
       <c r="M170" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N170" s="13">
         <v>2010</v>
@@ -9740,7 +9743,7 @@
         <v>382481.53</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D171" s="13">
         <v>10</v>
@@ -9768,7 +9771,7 @@
         <v>5.58</v>
       </c>
       <c r="M171" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N171" s="13">
         <v>2010</v>
@@ -9794,7 +9797,7 @@
         <v>5744150.3499999996</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D172" s="13">
         <v>1</v>
@@ -9822,7 +9825,7 @@
         <v>6.76</v>
       </c>
       <c r="M172" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N172" s="13">
         <v>2011</v>
@@ -9848,7 +9851,7 @@
         <v>1849110.07</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D173" s="13">
         <v>2</v>
@@ -9876,7 +9879,7 @@
         <v>6.27</v>
       </c>
       <c r="M173" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N173" s="13">
         <v>2011</v>
@@ -9902,7 +9905,7 @@
         <v>10306717.890000001</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D174" s="13">
         <v>3</v>
@@ -9930,7 +9933,7 @@
         <v>7.01</v>
       </c>
       <c r="M174" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N174" s="13">
         <v>2011</v>
@@ -9956,7 +9959,7 @@
         <v>2634128.0099999998</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D175" s="13">
         <v>4</v>
@@ -9984,7 +9987,7 @@
         <v>6.42</v>
       </c>
       <c r="M175" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N175" s="13">
         <v>2011</v>
@@ -10010,7 +10013,7 @@
         <v>3760802.93</v>
       </c>
       <c r="C176" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D176" s="13">
         <v>5</v>
@@ -10038,7 +10041,7 @@
         <v>6.58</v>
       </c>
       <c r="M176" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N176" s="13">
         <v>2011</v>
@@ -10064,7 +10067,7 @@
         <v>1750707.82</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D177" s="13">
         <v>6</v>
@@ -10092,7 +10095,7 @@
         <v>6.24</v>
       </c>
       <c r="M177" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N177" s="13">
         <v>2011</v>
@@ -10118,7 +10121,7 @@
         <v>4458310.62</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D178" s="13">
         <v>7</v>
@@ -10146,7 +10149,7 @@
         <v>6.65</v>
       </c>
       <c r="M178" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N178" s="13">
         <v>2011</v>
@@ -10172,7 +10175,7 @@
         <v>1288531.1399999999</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D179" s="13">
         <v>8</v>
@@ -10200,7 +10203,7 @@
         <v>6.11</v>
       </c>
       <c r="M179" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N179" s="13">
         <v>2011</v>
@@ -10226,7 +10229,7 @@
         <v>1000438.15</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D180" s="13">
         <v>9</v>
@@ -10254,7 +10257,7 @@
         <v>6</v>
       </c>
       <c r="M180" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N180" s="13">
         <v>2011</v>
@@ -10280,7 +10283,7 @@
         <v>452757.04</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D181" s="13">
         <v>10</v>
@@ -10308,7 +10311,7 @@
         <v>5.66</v>
       </c>
       <c r="M181" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N181" s="13">
         <v>2011</v>
@@ -10334,7 +10337,7 @@
         <v>5422822.2199999997</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D182" s="13">
         <v>1</v>
@@ -10362,7 +10365,7 @@
         <v>6.73</v>
       </c>
       <c r="M182" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N182" s="13">
         <v>2012</v>
@@ -10388,7 +10391,7 @@
         <v>1849384.71</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D183" s="13">
         <v>2</v>
@@ -10416,7 +10419,7 @@
         <v>6.27</v>
       </c>
       <c r="M183" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N183" s="13">
         <v>2012</v>
@@ -10442,7 +10445,7 @@
         <v>10569390.300000001</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D184" s="13">
         <v>3</v>
@@ -10470,7 +10473,7 @@
         <v>7.02</v>
       </c>
       <c r="M184" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N184" s="13">
         <v>2012</v>
@@ -10496,7 +10499,7 @@
         <v>2637700.09</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D185" s="13">
         <v>4</v>
@@ -10524,7 +10527,7 @@
         <v>6.42</v>
       </c>
       <c r="M185" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N185" s="13">
         <v>2012</v>
@@ -10550,7 +10553,7 @@
         <v>2954037.1</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D186" s="13">
         <v>5</v>
@@ -10578,7 +10581,7 @@
         <v>6.47</v>
       </c>
       <c r="M186" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N186" s="13">
         <v>2012</v>
@@ -10604,7 +10607,7 @@
         <v>1628479.68</v>
       </c>
       <c r="C187" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D187" s="13">
         <v>6</v>
@@ -10632,7 +10635,7 @@
         <v>6.21</v>
       </c>
       <c r="M187" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N187" s="13">
         <v>2012</v>
@@ -10658,7 +10661,7 @@
         <v>4050748.32</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D188" s="13">
         <v>7</v>
@@ -10686,7 +10689,7 @@
         <v>6.61</v>
       </c>
       <c r="M188" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N188" s="13">
         <v>2012</v>
@@ -10712,7 +10715,7 @@
         <v>1224190.46</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D189" s="13">
         <v>8</v>
@@ -10740,7 +10743,7 @@
         <v>6.09</v>
       </c>
       <c r="M189" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N189" s="13">
         <v>2012</v>
@@ -10766,7 +10769,7 @@
         <v>875380.83</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D190" s="13">
         <v>9</v>
@@ -10794,7 +10797,7 @@
         <v>5.94</v>
       </c>
       <c r="M190" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N190" s="13">
         <v>2012</v>
@@ -10820,7 +10823,7 @@
         <v>477763.29</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D191" s="13">
         <v>10</v>
@@ -10848,7 +10851,7 @@
         <v>5.68</v>
       </c>
       <c r="M191" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N191" s="13">
         <v>2012</v>
@@ -10874,7 +10877,7 @@
         <v>6030076.1200000001</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D192" s="13">
         <v>1</v>
@@ -10902,7 +10905,7 @@
         <v>6.78</v>
       </c>
       <c r="M192" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N192" s="13">
         <v>2013</v>
@@ -10928,7 +10931,7 @@
         <v>1884313.5</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D193" s="13">
         <v>2</v>
@@ -10956,7 +10959,7 @@
         <v>6.28</v>
       </c>
       <c r="M193" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N193" s="13">
         <v>2013</v>
@@ -10982,7 +10985,7 @@
         <v>10094012.09</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D194" s="13">
         <v>3</v>
@@ -11010,7 +11013,7 @@
         <v>7</v>
       </c>
       <c r="M194" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N194" s="13">
         <v>2013</v>
@@ -11036,7 +11039,7 @@
         <v>1892005.6</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D195" s="13">
         <v>4</v>
@@ -11064,7 +11067,7 @@
         <v>6.28</v>
       </c>
       <c r="M195" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N195" s="13">
         <v>2013</v>
@@ -11090,7 +11093,7 @@
         <v>2612661.5</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D196" s="13">
         <v>5</v>
@@ -11118,7 +11121,7 @@
         <v>6.42</v>
       </c>
       <c r="M196" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N196" s="13">
         <v>2013</v>
@@ -11144,7 +11147,7 @@
         <v>1245769.47</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D197" s="13">
         <v>6</v>
@@ -11172,7 +11175,7 @@
         <v>6.1</v>
       </c>
       <c r="M197" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N197" s="13">
         <v>2013</v>
@@ -11198,7 +11201,7 @@
         <v>3556173.29</v>
       </c>
       <c r="C198" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D198" s="13">
         <v>7</v>
@@ -11226,7 +11229,7 @@
         <v>6.55</v>
       </c>
       <c r="M198" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N198" s="13">
         <v>2013</v>
@@ -11252,7 +11255,7 @@
         <v>849928.95</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D199" s="13">
         <v>8</v>
@@ -11280,7 +11283,7 @@
         <v>5.93</v>
       </c>
       <c r="M199" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N199" s="13">
         <v>2013</v>
@@ -11306,7 +11309,7 @@
         <v>816758.23</v>
       </c>
       <c r="C200" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D200" s="13">
         <v>9</v>
@@ -11334,7 +11337,7 @@
         <v>5.91</v>
       </c>
       <c r="M200" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N200" s="13">
         <v>2013</v>
@@ -11360,7 +11363,7 @@
         <v>1574174.67</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D201" s="13">
         <v>10</v>
@@ -11388,7 +11391,7 @@
         <v>6.2</v>
       </c>
       <c r="M201" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N201" s="13">
         <v>2013</v>
@@ -11414,7 +11417,7 @@
         <v>6188368.2000000002</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D202" s="13">
         <v>1</v>
@@ -11442,7 +11445,7 @@
         <v>6.79</v>
       </c>
       <c r="M202" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N202" s="13">
         <v>2014</v>
@@ -11468,7 +11471,7 @@
         <v>1845857.89</v>
       </c>
       <c r="C203" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D203" s="13">
         <v>2</v>
@@ -11496,7 +11499,7 @@
         <v>6.27</v>
       </c>
       <c r="M203" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N203" s="13">
         <v>2014</v>
@@ -11522,7 +11525,7 @@
         <v>9722251.5199999996</v>
       </c>
       <c r="C204" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D204" s="13">
         <v>3</v>
@@ -11550,7 +11553,7 @@
         <v>6.99</v>
       </c>
       <c r="M204" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N204" s="13">
         <v>2014</v>
@@ -11576,7 +11579,7 @@
         <v>2101165.17</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D205" s="13">
         <v>4</v>
@@ -11604,7 +11607,7 @@
         <v>6.32</v>
       </c>
       <c r="M205" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N205" s="13">
         <v>2014</v>
@@ -11630,7 +11633,7 @@
         <v>2474718.81</v>
       </c>
       <c r="C206" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D206" s="13">
         <v>5</v>
@@ -11658,7 +11661,7 @@
         <v>6.39</v>
       </c>
       <c r="M206" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N206" s="13">
         <v>2014</v>
@@ -11684,7 +11687,7 @@
         <v>1248047.6499999999</v>
       </c>
       <c r="C207" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D207" s="13">
         <v>6</v>
@@ -11712,7 +11715,7 @@
         <v>6.1</v>
       </c>
       <c r="M207" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N207" s="13">
         <v>2014</v>
@@ -11738,7 +11741,7 @@
         <v>3493118.23</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D208" s="13">
         <v>7</v>
@@ -11766,7 +11769,7 @@
         <v>6.54</v>
       </c>
       <c r="M208" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N208" s="13">
         <v>2014</v>
@@ -11792,7 +11795,7 @@
         <v>947520.62</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D209" s="13">
         <v>8</v>
@@ -11820,7 +11823,7 @@
         <v>5.98</v>
       </c>
       <c r="M209" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N209" s="13">
         <v>2014</v>
@@ -11846,7 +11849,7 @@
         <v>806136.69</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D210" s="13">
         <v>9</v>
@@ -11874,7 +11877,7 @@
         <v>5.91</v>
       </c>
       <c r="M210" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N210" s="13">
         <v>2014</v>
@@ -11900,7 +11903,7 @@
         <v>1752794.62</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D211" s="13">
         <v>10</v>
@@ -11928,7 +11931,7 @@
         <v>6.24</v>
       </c>
       <c r="M211" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N211" s="13">
         <v>2014</v>
@@ -11954,7 +11957,7 @@
         <v>5270146.96</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D212" s="13">
         <v>1</v>
@@ -11982,7 +11985,7 @@
         <v>6.72</v>
       </c>
       <c r="M212" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N212" s="13">
         <v>2015</v>
@@ -12008,7 +12011,7 @@
         <v>1968713.05</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D213" s="13">
         <v>2</v>
@@ -12036,7 +12039,7 @@
         <v>6.29</v>
       </c>
       <c r="M213" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N213" s="13">
         <v>2015</v>
@@ -12062,7 +12065,7 @@
         <v>10679631.210000001</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D214" s="13">
         <v>3</v>
@@ -12090,7 +12093,7 @@
         <v>7.03</v>
       </c>
       <c r="M214" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N214" s="13">
         <v>2015</v>
@@ -12116,7 +12119,7 @@
         <v>2378890.4900000002</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D215" s="13">
         <v>4</v>
@@ -12144,7 +12147,7 @@
         <v>6.38</v>
       </c>
       <c r="M215" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N215" s="13">
         <v>2015</v>
@@ -12170,7 +12173,7 @@
         <v>2675517.65</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D216" s="13">
         <v>5</v>
@@ -12198,7 +12201,7 @@
         <v>6.43</v>
       </c>
       <c r="M216" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N216" s="13">
         <v>2015</v>
@@ -12224,7 +12227,7 @@
         <v>1093412.6000000001</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D217" s="13">
         <v>6</v>
@@ -12252,7 +12255,7 @@
         <v>6.04</v>
       </c>
       <c r="M217" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N217" s="13">
         <v>2015</v>
@@ -12278,7 +12281,7 @@
         <v>3500532.62</v>
       </c>
       <c r="C218" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D218" s="13">
         <v>7</v>
@@ -12306,7 +12309,7 @@
         <v>6.54</v>
       </c>
       <c r="M218" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N218" s="13">
         <v>2015</v>
@@ -12332,7 +12335,7 @@
         <v>1055420.73</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D219" s="13">
         <v>8</v>
@@ -12360,7 +12363,7 @@
         <v>6.02</v>
       </c>
       <c r="M219" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N219" s="13">
         <v>2015</v>
@@ -12386,7 +12389,7 @@
         <v>767781.93</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D220" s="13">
         <v>9</v>
@@ -12414,7 +12417,7 @@
         <v>5.89</v>
       </c>
       <c r="M220" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N220" s="13">
         <v>2015</v>
@@ -12440,7 +12443,7 @@
         <v>769735.11</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D221" s="13">
         <v>10</v>
@@ -12468,7 +12471,7 @@
         <v>5.89</v>
       </c>
       <c r="M221" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N221" s="13">
         <v>2015</v>
@@ -12494,7 +12497,7 @@
         <v>4561748.54</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D222" s="13">
         <v>1</v>
@@ -12522,7 +12525,7 @@
         <v>6.66</v>
       </c>
       <c r="M222" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N222" s="13">
         <v>2016</v>
@@ -12548,7 +12551,7 @@
         <v>2236346.44</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D223" s="13">
         <v>2</v>
@@ -12576,7 +12579,7 @@
         <v>6.35</v>
       </c>
       <c r="M223" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N223" s="13">
         <v>2016</v>
@@ -12602,7 +12605,7 @@
         <v>11304934</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D224" s="13">
         <v>3</v>
@@ -12630,7 +12633,7 @@
         <v>7.05</v>
       </c>
       <c r="M224" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N224" s="13">
         <v>2016</v>
@@ -12656,7 +12659,7 @@
         <v>2204994.86</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D225" s="13">
         <v>4</v>
@@ -12684,7 +12687,7 @@
         <v>6.34</v>
       </c>
       <c r="M225" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N225" s="13">
         <v>2016</v>
@@ -12710,7 +12713,7 @@
         <v>2659103.84</v>
       </c>
       <c r="C226" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D226" s="13">
         <v>5</v>
@@ -12738,7 +12741,7 @@
         <v>6.42</v>
       </c>
       <c r="M226" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N226" s="13">
         <v>2016</v>
@@ -12764,7 +12767,7 @@
         <v>1180484.96</v>
       </c>
       <c r="C227" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D227" s="13">
         <v>6</v>
@@ -12792,7 +12795,7 @@
         <v>6.07</v>
       </c>
       <c r="M227" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N227" s="13">
         <v>2016</v>
@@ -12818,7 +12821,7 @@
         <v>3164432.08</v>
       </c>
       <c r="C228" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D228" s="13">
         <v>7</v>
@@ -12846,7 +12849,7 @@
         <v>6.5</v>
       </c>
       <c r="M228" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N228" s="13">
         <v>2016</v>
@@ -12872,7 +12875,7 @@
         <v>939780.59</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D229" s="13">
         <v>8</v>
@@ -12900,7 +12903,7 @@
         <v>5.97</v>
       </c>
       <c r="M229" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N229" s="13">
         <v>2016</v>
@@ -12926,7 +12929,7 @@
         <v>846944.63</v>
       </c>
       <c r="C230" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D230" s="13">
         <v>9</v>
@@ -12954,7 +12957,7 @@
         <v>5.93</v>
       </c>
       <c r="M230" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N230" s="13">
         <v>2016</v>
@@ -12980,7 +12983,7 @@
         <v>1355278.34</v>
       </c>
       <c r="C231" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D231" s="13">
         <v>10</v>
@@ -13008,7 +13011,7 @@
         <v>6.13</v>
       </c>
       <c r="M231" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N231" s="13">
         <v>2016</v>
@@ -13034,7 +13037,7 @@
         <v>5484913.54</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D232" s="13">
         <v>1</v>
@@ -13062,7 +13065,7 @@
         <v>6.74</v>
       </c>
       <c r="M232" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N232" s="13">
         <v>2017</v>
@@ -13088,7 +13091,7 @@
         <v>2498806.7200000002</v>
       </c>
       <c r="C233" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D233" s="13">
         <v>2</v>
@@ -13116,7 +13119,7 @@
         <v>6.4</v>
       </c>
       <c r="M233" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N233" s="13">
         <v>2017</v>
@@ -13142,7 +13145,7 @@
         <v>11752632.800000001</v>
       </c>
       <c r="C234" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D234" s="13">
         <v>3</v>
@@ -13170,7 +13173,7 @@
         <v>7.07</v>
       </c>
       <c r="M234" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N234" s="13">
         <v>2017</v>
@@ -13196,7 +13199,7 @@
         <v>3889342.35</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D235" s="13">
         <v>4</v>
@@ -13224,7 +13227,7 @@
         <v>6.59</v>
       </c>
       <c r="M235" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N235" s="13">
         <v>2017</v>
@@ -13250,7 +13253,7 @@
         <v>2851736.08</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D236" s="13">
         <v>5</v>
@@ -13278,7 +13281,7 @@
         <v>6.46</v>
       </c>
       <c r="M236" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N236" s="13">
         <v>2017</v>
@@ -13304,7 +13307,7 @@
         <v>2807758.02</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D237" s="13">
         <v>6</v>
@@ -13332,7 +13335,7 @@
         <v>6.45</v>
       </c>
       <c r="M237" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N237" s="13">
         <v>2017</v>
@@ -13358,7 +13361,7 @@
         <v>3449747.79</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D238" s="13">
         <v>7</v>
@@ -13386,7 +13389,7 @@
         <v>6.54</v>
       </c>
       <c r="M238" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N238" s="13">
         <v>2017</v>
@@ -13412,7 +13415,7 @@
         <v>939016.49</v>
       </c>
       <c r="C239" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D239" s="13">
         <v>8</v>
@@ -13440,7 +13443,7 @@
         <v>5.97</v>
       </c>
       <c r="M239" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N239" s="13">
         <v>2017</v>
@@ -13466,7 +13469,7 @@
         <v>905337.09</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D240" s="13">
         <v>9</v>
@@ -13494,7 +13497,7 @@
         <v>5.96</v>
       </c>
       <c r="M240" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N240" s="13">
         <v>2017</v>
@@ -13520,7 +13523,7 @@
         <v>2530724.9500000002</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D241" s="13">
         <v>10</v>
@@ -13548,7 +13551,7 @@
         <v>6.4</v>
       </c>
       <c r="M241" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N241" s="13">
         <v>2017</v>
@@ -13574,7 +13577,7 @@
         <v>5854664.1500000004</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D242" s="13">
         <v>1</v>
@@ -13602,7 +13605,7 @@
         <v>6.77</v>
       </c>
       <c r="M242" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N242" s="13">
         <v>2018</v>
@@ -13628,7 +13631,7 @@
         <v>2860166.84</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D243" s="13">
         <v>2</v>
@@ -13656,7 +13659,7 @@
         <v>6.46</v>
       </c>
       <c r="M243" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N243" s="13">
         <v>2018</v>
@@ -13682,7 +13685,7 @@
         <v>13483750.189999999</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D244" s="13">
         <v>3</v>
@@ -13710,7 +13713,7 @@
         <v>7.13</v>
       </c>
       <c r="M244" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N244" s="13">
         <v>2018</v>
@@ -13736,7 +13739,7 @@
         <v>8091866.6100000003</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D245" s="13">
         <v>4</v>
@@ -13764,7 +13767,7 @@
         <v>6.91</v>
       </c>
       <c r="M245" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N245" s="13">
         <v>2018</v>
@@ -13790,7 +13793,7 @@
         <v>3633161.6</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D246" s="13">
         <v>5</v>
@@ -13818,7 +13821,7 @@
         <v>6.56</v>
       </c>
       <c r="M246" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N246" s="13">
         <v>2018</v>
@@ -13844,7 +13847,7 @@
         <v>6656137.3600000003</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D247" s="13">
         <v>6</v>
@@ -13872,7 +13875,7 @@
         <v>6.82</v>
       </c>
       <c r="M247" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N247" s="13">
         <v>2018</v>
@@ -13898,7 +13901,7 @@
         <v>3750588.13</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D248" s="13">
         <v>7</v>
@@ -13926,7 +13929,7 @@
         <v>6.57</v>
       </c>
       <c r="M248" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N248" s="13">
         <v>2018</v>
@@ -13952,7 +13955,7 @@
         <v>1431484.03</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D249" s="13">
         <v>8</v>
@@ -13980,7 +13983,7 @@
         <v>6.16</v>
       </c>
       <c r="M249" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N249" s="13">
         <v>2018</v>
@@ -14006,7 +14009,7 @@
         <v>1086582.32</v>
       </c>
       <c r="C250" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D250" s="13">
         <v>9</v>
@@ -14034,7 +14037,7 @@
         <v>6.04</v>
       </c>
       <c r="M250" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N250" s="13">
         <v>2018</v>
@@ -14060,7 +14063,7 @@
         <v>3574383.35</v>
       </c>
       <c r="C251" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D251" s="13">
         <v>10</v>
@@ -14088,7 +14091,7 @@
         <v>6.55</v>
       </c>
       <c r="M251" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N251" s="13">
         <v>2018</v>
@@ -14114,7 +14117,7 @@
         <v>6795588.25</v>
       </c>
       <c r="C252" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D252" s="13">
         <v>1</v>
@@ -14142,7 +14145,7 @@
         <v>6.83</v>
       </c>
       <c r="M252" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N252" s="13">
         <v>2019</v>
@@ -14168,7 +14171,7 @@
         <v>3065656.47</v>
       </c>
       <c r="C253" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D253" s="13">
         <v>2</v>
@@ -14196,7 +14199,7 @@
         <v>6.49</v>
       </c>
       <c r="M253" s="13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N253" s="13">
         <v>2019</v>
@@ -14222,7 +14225,7 @@
         <v>12372622.189999999</v>
       </c>
       <c r="C254" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D254" s="13">
         <v>3</v>
@@ -14250,7 +14253,7 @@
         <v>7.09</v>
       </c>
       <c r="M254" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="N254" s="13">
         <v>2019</v>
@@ -14276,7 +14279,7 @@
         <v>10135818.98</v>
       </c>
       <c r="C255" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D255" s="13">
         <v>4</v>
@@ -14304,7 +14307,7 @@
         <v>7.01</v>
       </c>
       <c r="M255" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N255" s="13">
         <v>2019</v>
@@ -14330,7 +14333,7 @@
         <v>4045851.72</v>
       </c>
       <c r="C256" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D256" s="13">
         <v>5</v>
@@ -14358,7 +14361,7 @@
         <v>6.61</v>
       </c>
       <c r="M256" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N256" s="13">
         <v>2019</v>
@@ -14384,7 +14387,7 @@
         <v>8260695.2999999998</v>
       </c>
       <c r="C257" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D257" s="13">
         <v>6</v>
@@ -14412,7 +14415,7 @@
         <v>6.92</v>
       </c>
       <c r="M257" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N257" s="13">
         <v>2019</v>
@@ -14438,7 +14441,7 @@
         <v>3936170.15</v>
       </c>
       <c r="C258" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D258" s="13">
         <v>7</v>
@@ -14466,7 +14469,7 @@
         <v>6.6</v>
       </c>
       <c r="M258" s="13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N258" s="13">
         <v>2019</v>
@@ -14492,7 +14495,7 @@
         <v>1565224.22</v>
       </c>
       <c r="C259" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D259" s="13">
         <v>8</v>
@@ -14520,7 +14523,7 @@
         <v>6.19</v>
       </c>
       <c r="M259" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N259" s="13">
         <v>2019</v>
@@ -14546,7 +14549,7 @@
         <v>1122648.5900000001</v>
       </c>
       <c r="C260" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D260" s="13">
         <v>9</v>
@@ -14574,7 +14577,7 @@
         <v>6.05</v>
       </c>
       <c r="M260" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N260" s="13">
         <v>2019</v>
@@ -14600,7 +14603,7 @@
         <v>3077149.42</v>
       </c>
       <c r="C261" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D261" s="13">
         <v>10</v>
@@ -14628,7 +14631,7 @@
         <v>6.49</v>
       </c>
       <c r="M261" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N261" s="13">
         <v>2019</v>

</xml_diff>